<commit_message>
Testcases for story 1.1.5
</commit_message>
<xml_diff>
--- a/1.1.5/Registration/Registration_Client_testcases.xlsx
+++ b/1.1.5/Registration/Registration_Client_testcases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP-10804" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="MOSIP-11295" sheetId="3" r:id="rId3"/>
     <sheet name="MOSIP-11474" sheetId="4" r:id="rId4"/>
     <sheet name="MOSIP-11510" sheetId="5" r:id="rId5"/>
+    <sheet name="MOSIP-11446" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="105">
   <si>
     <t xml:space="preserve">TestCase_No </t>
   </si>
@@ -295,6 +296,54 @@
   </si>
   <si>
     <t>The packet should contain all the data and should be processed easily  without any failure</t>
+  </si>
+  <si>
+    <t>Registration Client_Onboarding_01</t>
+  </si>
+  <si>
+    <t>Onboarding</t>
+  </si>
+  <si>
+    <t>To onboard user and check whether the data is saved in Local DB</t>
+  </si>
+  <si>
+    <t>The data should be saved in DB in bio metric templates format under BIO_ISO_IMAGE Column of reg.USER_BIOMETRIC</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Registration Client_Onboarding_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onboard Multiple User from a machine and check the local DB </t>
+  </si>
+  <si>
+    <t>The reg.USER_BIOMETRIC table should contain details of all the onboarded user in DB Table.</t>
+  </si>
+  <si>
+    <t>Registration Client_Onboarding_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create a packet and see whether the packet is getting created </t>
+  </si>
+  <si>
+    <t>The packet should be created successfully.</t>
+  </si>
+  <si>
+    <t>Registration Client_Onboarding_04</t>
+  </si>
+  <si>
+    <t>Update the Biometric of user and check in user DB that new Biometric Modality is present or not</t>
+  </si>
+  <si>
+    <t>The table should contain the added Modality in the BIO_ISO_IMAGE Column of reg.USER_BIOMETRIC</t>
+  </si>
+  <si>
+    <t>Registration Client_Onboarding_05</t>
+  </si>
+  <si>
+    <t>Update Modality and Onboard new user and check the DB</t>
   </si>
 </sst>
 </file>
@@ -655,7 +704,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1405,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,4 +1617,180 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
+      <formula1>"Admin, Credential Services, IDA, Partner Mgmt, Pre Registration, Registration Client, Registration Processor, Resident Services"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H6">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
+      <formula1>"Acceptance, Functional, Smoke, Security, Performance"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>